<commit_message>
Updated ECCC PPT and some minor code fixes
</commit_message>
<xml_diff>
--- a/Docs/Vortex Packets.xlsx
+++ b/Docs/Vortex Packets.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="101">
   <si>
     <t>Byte#</t>
   </si>
@@ -54,39 +54,21 @@
     <t>X Speed (Low Byte)</t>
   </si>
   <si>
-    <t>X Speed (High Byte)</t>
-  </si>
-  <si>
     <t>Y Speed (Low Byte)</t>
   </si>
   <si>
-    <t>Y Speed (High Byte)</t>
-  </si>
-  <si>
     <t>Sprite Color</t>
   </si>
   <si>
     <t>Sprite Number</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>C64 to Server</t>
   </si>
   <si>
     <t>C64 Listens on Port 3000</t>
   </si>
   <si>
-    <t>Checksum</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
-    <t>Revised June 4, 2008</t>
-  </si>
-  <si>
     <t>Server Listens on Port 3005</t>
   </si>
   <si>
@@ -297,75 +279,12 @@
     <t>SOUNDS</t>
   </si>
   <si>
-    <t>Begin playing Sound Effect #1</t>
-  </si>
-  <si>
     <t>Begin playing Sound Effect #2</t>
   </si>
   <si>
     <t>Begin playing Sound Effect #3</t>
   </si>
   <si>
-    <t>Begin playing Sound Effect #4</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #5</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #6</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #7</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #8</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #9</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #10</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #11</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #12</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #13</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #14</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #15</t>
-  </si>
-  <si>
-    <t>Begin playing Sound Effect #16</t>
-  </si>
-  <si>
-    <t>Laser Shot</t>
-  </si>
-  <si>
-    <t>Explosion</t>
-  </si>
-  <si>
-    <t>Powerup</t>
-  </si>
-  <si>
-    <t>Mine Drop</t>
-  </si>
-  <si>
-    <t>etc.</t>
-  </si>
-  <si>
-    <t>SCREEN DATA - MAX LENGTH 1000</t>
-  </si>
-  <si>
-    <t>Sprite location and type data.  Sprite 0 is always the player (highlest priority).    Server may multiplex these if more than 8 entities on screen.</t>
-  </si>
-  <si>
     <t>CHECKSUM (Future??)</t>
   </si>
   <si>
@@ -382,6 +301,33 @@
   </si>
   <si>
     <t>TBD.</t>
+  </si>
+  <si>
+    <t>Signed</t>
+  </si>
+  <si>
+    <t>Sprite location and type data.  Sprite 0 is always the player (highest priority).    Server may multiplex these if more than 8 entities on screen.  Or, show 8 closest objects to player.</t>
+  </si>
+  <si>
+    <t>1=Laser Shot</t>
+  </si>
+  <si>
+    <t>2=Explosion</t>
+  </si>
+  <si>
+    <t>3=Powerup</t>
+  </si>
+  <si>
+    <t>4-Mine Drop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Begin playing Sound Effect #1  </t>
+  </si>
+  <si>
+    <t>Expansion for more sound data.</t>
+  </si>
+  <si>
+    <t>SCREEN DATA - MAX LENGTH  800</t>
   </si>
 </sst>
 </file>
@@ -562,9 +508,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -586,6 +529,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
@@ -1293,23 +1239,23 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.15">
       <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1320,22 +1266,22 @@
       <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>50</v>
+      <c r="C5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>23</v>
+      <c r="C6" s="16" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.15">
@@ -1427,146 +1373,146 @@
         <v>16</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B22" s="11"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B23" s="1">
         <v>0</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
+      <c r="C23" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
+      <c r="C24" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B25" s="11"/>
-      <c r="C25" s="13"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="12"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B26" s="1">
         <v>0</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
+      <c r="C26" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B27" s="1">
         <v>1</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
+      <c r="C27" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B28" s="1">
         <v>2</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
+        <v>27</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B29" s="1">
         <v>3</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
+      <c r="C29" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B30" s="1">
         <v>4</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
+      <c r="C30" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B31" s="1">
@@ -1575,57 +1521,63 @@
       <c r="C31" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H31" s="13"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
+      <c r="D31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="12"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B32" s="1">
         <v>6</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="18">
+        <v>9</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="17">
         <v>8</v>
       </c>
-      <c r="H32" s="18">
+      <c r="H32" s="17">
         <v>1</v>
       </c>
-      <c r="I32" s="21">
+      <c r="I32" s="20">
         <v>2</v>
       </c>
-      <c r="J32" s="11"/>
+      <c r="J32" s="10"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B33" s="1">
         <v>7</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="18">
+        <v>31</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="17">
         <v>7</v>
       </c>
-      <c r="H33" s="18">
+      <c r="H33" s="17">
         <v>0</v>
       </c>
-      <c r="I33" s="21">
+      <c r="I33" s="20">
         <v>3</v>
       </c>
-      <c r="J33" s="13" t="s">
-        <v>45</v>
+      <c r="J33" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.15">
@@ -1633,392 +1585,392 @@
         <v>8</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="18">
+        <v>33</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="17">
         <v>6</v>
       </c>
-      <c r="H34" s="18">
+      <c r="H34" s="17">
         <v>5</v>
       </c>
-      <c r="I34" s="21">
+      <c r="I34" s="20">
         <v>4</v>
       </c>
-      <c r="J34" s="11"/>
+      <c r="J34" s="10"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B35" s="1">
         <v>9</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
+        <v>35</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B36" s="1">
         <v>10</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
+        <v>36</v>
+      </c>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B37" s="1">
         <v>11</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
+        <v>40</v>
+      </c>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B38" s="1">
         <v>12</v>
       </c>
       <c r="C38" s="6"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B39" s="1">
         <v>13</v>
       </c>
       <c r="C39" s="6"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B40" s="1">
         <v>14</v>
       </c>
       <c r="C40" s="6"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B41" s="1">
         <v>15</v>
       </c>
       <c r="C41" s="6"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B42" s="1">
         <v>16</v>
       </c>
       <c r="C42" s="8"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B43" s="11"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B44" s="11"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B55" s="11"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B56" s="11"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="11"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="10"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B67" s="11"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="11"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="10"/>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B68" s="11"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="11"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="10"/>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B72" s="11"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B75" s="11"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="D76" s="11"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="D77" s="11"/>
+      <c r="D77" s="10"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="D78" s="11"/>
+      <c r="D78" s="10"/>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="D79" s="11"/>
+      <c r="D79" s="10"/>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="D80" s="11"/>
+      <c r="D80" s="10"/>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D81" s="11"/>
+      <c r="D81" s="10"/>
     </row>
     <row r="82" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D82" s="11"/>
+      <c r="D82" s="10"/>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D83" s="11"/>
+      <c r="D83" s="10"/>
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D84" s="11"/>
+      <c r="D84" s="10"/>
     </row>
     <row r="85" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D85" s="11"/>
+      <c r="D85" s="10"/>
     </row>
     <row r="86" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D86" s="11"/>
+      <c r="D86" s="10"/>
     </row>
     <row r="87" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D87" s="11"/>
+      <c r="D87" s="10"/>
     </row>
     <row r="88" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D88" s="11"/>
+      <c r="D88" s="10"/>
     </row>
     <row r="89" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D89" s="11"/>
+      <c r="D89" s="10"/>
     </row>
     <row r="90" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D90" s="11"/>
+      <c r="D90" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2030,8 +1982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D140" sqref="D140"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
@@ -2424,10 +2376,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C1" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -2445,25 +2397,25 @@
       <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>51</v>
+      <c r="C4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>53</v>
+      <c r="C5" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -2479,88 +2431,88 @@
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B9" s="11"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="11"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="1">
         <v>0</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>54</v>
+      <c r="C10" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="11"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>55</v>
+      <c r="C11" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="11"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="11"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="1">
         <v>3</v>
       </c>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="11"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="1">
         <v>0</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>57</v>
+      <c r="C16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A17" s="11"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>58</v>
+      <c r="C17" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
@@ -2568,7 +2520,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
@@ -2577,404 +2529,330 @@
       </c>
       <c r="C19" s="6"/>
     </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+    </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="K22" s="1">
-        <v>14</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B23" s="1">
         <v>0</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="K23" s="1">
-        <v>15</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="C23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
     </row>
     <row r="24" spans="1:14" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>68</v>
+      <c r="C24" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="K24" s="1">
-        <v>16</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="K25" s="1">
-        <v>17</v>
-      </c>
-      <c r="L25" s="7" t="s">
-        <v>8</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="10"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B26" s="1">
         <v>3</v>
       </c>
       <c r="C26" s="6"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="K26" s="1">
-        <v>18</v>
-      </c>
-      <c r="L26" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="10"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="K27" s="1">
-        <v>19</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B28" s="1">
         <v>0</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="K28" s="1">
-        <v>20</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M28" s="9"/>
+      <c r="C28" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="28"/>
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="K29" s="1">
-        <v>21</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
+      <c r="E29" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="9"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B30" s="1">
         <v>2</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="K30" s="1">
-        <v>22</v>
-      </c>
-      <c r="L30" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
+        <v>54</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B31" s="1">
         <v>3</v>
       </c>
       <c r="C31" s="6"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="K31" s="1">
-        <v>23</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="9"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="K32" s="1">
-        <v>24</v>
-      </c>
-      <c r="L32" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="9"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="K33" s="1">
-        <v>25</v>
-      </c>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="9"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B34" s="1">
         <v>0</v>
       </c>
-      <c r="C34" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="K34" s="1">
-        <v>26</v>
-      </c>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
+      <c r="C34" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="9"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B35" s="1">
         <v>1</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="K35" s="1">
-        <v>27</v>
-      </c>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
+      <c r="E35" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="9"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B36" s="1">
         <v>2</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="K36" s="1">
-        <v>28</v>
-      </c>
-      <c r="M36" s="10"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="12"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B37" s="1">
         <v>3</v>
       </c>
       <c r="C37" s="6"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="K37" s="1">
-        <v>29</v>
-      </c>
-      <c r="L37" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="M37" s="10"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="K38" s="1">
-        <v>30</v>
-      </c>
-      <c r="L38" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M38" s="10"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="K39" s="1">
-        <v>31</v>
-      </c>
-      <c r="L39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="9"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="K40" s="1">
-        <v>32</v>
-      </c>
-      <c r="L40" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="9"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B41" s="1">
         <v>0</v>
       </c>
-      <c r="C41" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="K41" s="1">
-        <v>33</v>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
+      <c r="C41" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="9"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B42" s="1">
         <v>1</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="24"/>
-      <c r="K42" s="1">
-        <v>34</v>
-      </c>
-      <c r="L42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="23"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="12"/>
+      <c r="N42" s="9"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B43" s="1">
         <v>2</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="K43" s="1">
-        <v>35</v>
-      </c>
-      <c r="L43" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M43" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="12"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B44" s="1">
         <v>3</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="K44" s="1">
-        <v>36</v>
-      </c>
-      <c r="L44" s="8" t="s">
-        <v>14</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B45" s="1">
         <v>4</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="K45" s="1">
-        <v>37</v>
-      </c>
-      <c r="L45" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="C45" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B46" s="1">
         <v>5</v>
       </c>
-      <c r="C46" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="K46" s="1">
-        <v>38</v>
-      </c>
-      <c r="L46" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="C46" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A47" s="10" t="s">
-        <v>80</v>
+      <c r="A47" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="B47" s="1">
         <v>6</v>
@@ -2982,18 +2860,15 @@
       <c r="C47" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="K47" s="1">
-        <v>39</v>
-      </c>
-      <c r="L47" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="D47" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B48" s="1">
@@ -3002,134 +2877,104 @@
       <c r="C48" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K48" s="1">
-        <v>40</v>
-      </c>
-      <c r="L48" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B49" s="1">
         <v>8</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K49" s="1">
-        <v>41</v>
-      </c>
-      <c r="L49" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K49" s="10"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="10"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B50" s="1">
         <v>9</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K50" s="1">
-        <v>42</v>
-      </c>
-      <c r="L50" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K50" s="10"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="10"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B51" s="1">
         <v>10</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K51" s="1">
-        <v>43</v>
-      </c>
-      <c r="L51" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B52" s="1">
         <v>11</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K52" s="1">
-        <v>44</v>
-      </c>
-      <c r="L52" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.15">
+        <v>9</v>
+      </c>
+      <c r="K52" s="10"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B53" s="1">
         <v>12</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K53" s="1">
-        <v>45</v>
-      </c>
-      <c r="L53" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.15">
+        <v>10</v>
+      </c>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B54" s="1">
         <v>13</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K54" s="1">
-        <v>46</v>
-      </c>
-      <c r="L54" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.15">
+        <v>11</v>
+      </c>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B55" s="1">
         <v>14</v>
       </c>
-      <c r="C55" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="K55" s="1">
-        <v>47</v>
-      </c>
-      <c r="L55" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C55" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="K55" s="10"/>
+      <c r="L55" s="10"/>
+      <c r="M55" s="10"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B56" s="1">
         <v>15</v>
       </c>
-      <c r="C56" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="K56" s="1">
-        <v>48</v>
-      </c>
-      <c r="L56" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A57" s="10" t="s">
-        <v>82</v>
+      <c r="C56" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="K56" s="10"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="10"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A57" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="B57" s="1">
         <v>16</v>
@@ -3137,145 +2982,115 @@
       <c r="C57" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K57" s="1">
-        <v>49</v>
-      </c>
-      <c r="L57" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K57" s="10"/>
+      <c r="L57" s="10"/>
+      <c r="M57" s="10"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B58" s="1">
         <v>17</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K58" s="1">
-        <v>50</v>
-      </c>
-      <c r="L58" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="10"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B59" s="1">
         <v>18</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K59" s="1">
-        <v>51</v>
-      </c>
-      <c r="L59" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+      <c r="M59" s="10"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B60" s="1">
         <v>19</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="D60" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K60" s="1">
-        <v>52</v>
-      </c>
-      <c r="L60" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="10"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B61" s="1">
         <v>20</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K61" s="1">
-        <v>53</v>
-      </c>
-      <c r="L61" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K61" s="10"/>
+      <c r="L61" s="12"/>
+      <c r="M61" s="10"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B62" s="1">
         <v>21</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K62" s="1">
-        <v>54</v>
-      </c>
-      <c r="L62" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K62" s="10"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="10"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B63" s="1">
         <v>22</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K63" s="1">
-        <v>55</v>
-      </c>
-      <c r="L63" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="K63" s="10"/>
+      <c r="L63" s="10"/>
+      <c r="M63" s="10"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B64" s="1">
         <v>23</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K64" s="1">
-        <v>56</v>
-      </c>
-      <c r="L64" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
+      <c r="M64" s="10"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B65" s="1">
         <v>24</v>
       </c>
-      <c r="C65" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="K65" s="1">
-        <v>57</v>
-      </c>
-      <c r="L65" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C65" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
+      <c r="M65" s="10"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B66" s="1">
         <v>25</v>
       </c>
-      <c r="C66" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="K66" s="1">
-        <v>58</v>
-      </c>
-      <c r="L66" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A67" s="10" t="s">
-        <v>83</v>
+      <c r="C66" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="10"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A67" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="B67" s="1">
         <v>26</v>
@@ -3283,145 +3098,115 @@
       <c r="C67" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K67" s="1">
-        <v>59</v>
-      </c>
-      <c r="L67" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B68" s="1">
         <v>27</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K68" s="1">
-        <v>60</v>
-      </c>
-      <c r="L68" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K68" s="10"/>
+      <c r="L68" s="10"/>
+      <c r="M68" s="10"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B69" s="1">
         <v>28</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K69" s="1">
-        <v>61</v>
-      </c>
-      <c r="L69" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B70" s="1">
         <v>29</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D70" s="10" t="s">
+      <c r="D70" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K70" s="1">
-        <v>62</v>
-      </c>
-      <c r="L70" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K70" s="10"/>
+      <c r="L70" s="10"/>
+      <c r="M70" s="10"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B71" s="1">
         <v>30</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K71" s="1">
-        <v>63</v>
-      </c>
-      <c r="L71" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K71" s="10"/>
+      <c r="L71" s="10"/>
+      <c r="M71" s="10"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B72" s="1">
         <v>31</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K72" s="1">
-        <v>64</v>
-      </c>
-      <c r="L72" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
+        <v>9</v>
+      </c>
+      <c r="K72" s="10"/>
+      <c r="L72" s="10"/>
+      <c r="M72" s="10"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B73" s="1">
         <v>32</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K73" s="1">
-        <v>65</v>
-      </c>
-      <c r="L73" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
+        <v>10</v>
+      </c>
+      <c r="K73" s="10"/>
+      <c r="L73" s="12"/>
+      <c r="M73" s="10"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B74" s="1">
         <v>33</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K74" s="1">
-        <v>66</v>
-      </c>
-      <c r="L74" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.15">
+        <v>11</v>
+      </c>
+      <c r="K74" s="10"/>
+      <c r="L74" s="12"/>
+      <c r="M74" s="10"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B75" s="1">
         <v>34</v>
       </c>
-      <c r="C75" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="K75" s="1">
-        <v>67</v>
-      </c>
-      <c r="L75" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C75" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+      <c r="M75" s="10"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B76" s="1">
         <v>35</v>
       </c>
-      <c r="C76" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="K76" s="1">
-        <v>68</v>
-      </c>
-      <c r="L76" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A77" s="10" t="s">
-        <v>84</v>
+      <c r="C76" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="K76" s="10"/>
+      <c r="L76" s="10"/>
+      <c r="M76" s="10"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A77" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="B77" s="1">
         <v>36</v>
@@ -3429,57 +3214,45 @@
       <c r="C77" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K77" s="1">
-        <v>69</v>
-      </c>
-      <c r="L77" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K77" s="10"/>
+      <c r="L77" s="10"/>
+      <c r="M77" s="10"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B78" s="1">
         <v>37</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K78" s="1">
-        <v>70</v>
-      </c>
-      <c r="L78" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K78" s="10"/>
+      <c r="L78" s="10"/>
+      <c r="M78" s="10"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B79" s="1">
         <v>38</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K79" s="1">
-        <v>71</v>
-      </c>
-      <c r="L79" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K79" s="10"/>
+      <c r="L79" s="10"/>
+      <c r="M79" s="10"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B80" s="1">
         <v>39</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D80" s="10" t="s">
+      <c r="D80" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K80" s="1">
-        <v>72</v>
-      </c>
-      <c r="L80" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="K80" s="10"/>
+      <c r="L80" s="10"/>
+      <c r="M80" s="10"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B81" s="1">
@@ -3488,86 +3261,68 @@
       <c r="C81" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K81" s="1">
-        <v>73</v>
-      </c>
-      <c r="L81" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="K81" s="10"/>
+      <c r="L81" s="10"/>
+      <c r="M81" s="10"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B82" s="1">
         <v>41</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K82" s="1">
-        <v>74</v>
-      </c>
-      <c r="L82" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="K82" s="10"/>
+      <c r="L82" s="10"/>
+      <c r="M82" s="10"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B83" s="1">
         <v>42</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K83" s="1">
-        <v>75</v>
-      </c>
-      <c r="L83" s="6" t="s">
-        <v>6</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="K83" s="10"/>
+      <c r="L83" s="10"/>
+      <c r="M83" s="10"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B84" s="1">
         <v>43</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K84" s="1">
-        <v>76</v>
-      </c>
-      <c r="L84" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="K84" s="10"/>
+      <c r="L84" s="10"/>
+      <c r="M84" s="10"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B85" s="1">
         <v>44</v>
       </c>
-      <c r="C85" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="K85" s="1">
-        <v>77</v>
-      </c>
-      <c r="L85" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="C85" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="K85" s="10"/>
+      <c r="L85" s="12"/>
+      <c r="M85" s="10"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B86" s="1">
         <v>45</v>
       </c>
-      <c r="C86" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="K86" s="1">
-        <v>78</v>
-      </c>
-      <c r="L86" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="C86" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="K86" s="10"/>
+      <c r="L86" s="12"/>
+      <c r="M86" s="10"/>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A87" s="10" t="s">
-        <v>85</v>
+      <c r="A87" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="B87" s="1">
         <v>46</v>
@@ -3575,12 +3330,9 @@
       <c r="C87" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K87" s="1">
-        <v>79</v>
-      </c>
-      <c r="L87" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="K87" s="10"/>
+      <c r="L87" s="10"/>
+      <c r="M87" s="10"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B88" s="1">
@@ -3589,12 +3341,9 @@
       <c r="C88" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K88" s="1">
-        <v>80</v>
-      </c>
-      <c r="L88" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="K88" s="10"/>
+      <c r="L88" s="10"/>
+      <c r="M88" s="10"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B89" s="1">
@@ -3603,12 +3352,9 @@
       <c r="C89" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K89" s="1">
-        <v>81</v>
-      </c>
-      <c r="L89" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
+      <c r="M89" s="10"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B90" s="1">
@@ -3617,15 +3363,12 @@
       <c r="C90" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D90" s="10" t="s">
+      <c r="D90" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K90" s="1">
-        <v>82</v>
-      </c>
-      <c r="L90" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+      <c r="M90" s="10"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B91" s="1">
@@ -3634,71 +3377,62 @@
       <c r="C91" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K91" s="1">
-        <v>83</v>
-      </c>
-      <c r="L91" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
+      <c r="M91" s="10"/>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B92" s="1">
         <v>51</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K92" s="1">
-        <v>84</v>
-      </c>
-      <c r="L92" s="8" t="s">
-        <v>14</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="K92" s="10"/>
+      <c r="L92" s="10"/>
+      <c r="M92" s="10"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B93" s="1">
         <v>52</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K93" s="1">
-        <v>85</v>
-      </c>
-      <c r="L93" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M93" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="K93" s="10"/>
+      <c r="L93" s="10"/>
+      <c r="M93" s="10"/>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B94" s="1">
         <v>53</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
+      <c r="M94" s="10"/>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B95" s="1">
         <v>54</v>
       </c>
-      <c r="C95" s="26" t="s">
-        <v>81</v>
+      <c r="C95" s="25" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B96" s="1">
         <v>55</v>
       </c>
-      <c r="C96" s="27" t="s">
-        <v>81</v>
+      <c r="C96" s="26" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A97" s="10" t="s">
-        <v>86</v>
+      <c r="A97" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="B97" s="1">
         <v>56</v>
@@ -3730,7 +3464,7 @@
       <c r="C100" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D100" s="10" t="s">
+      <c r="D100" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3747,7 +3481,7 @@
         <v>61</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.15">
@@ -3755,7 +3489,7 @@
         <v>62</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.15">
@@ -3763,28 +3497,28 @@
         <v>63</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B105" s="1">
         <v>64</v>
       </c>
-      <c r="C105" s="26" t="s">
-        <v>81</v>
+      <c r="C105" s="25" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B106" s="1">
         <v>65</v>
       </c>
-      <c r="C106" s="27" t="s">
+      <c r="C106" s="26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A107" s="9" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A107" s="10" t="s">
-        <v>87</v>
       </c>
       <c r="B107" s="1">
         <v>66</v>
@@ -3816,7 +3550,7 @@
       <c r="C110" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D110" s="10" t="s">
+      <c r="D110" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3833,199 +3567,177 @@
         <v>71</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B113" s="1">
         <v>72</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B114" s="1">
         <v>73</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B115" s="1">
         <v>74</v>
       </c>
-      <c r="C115" s="26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C115" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B116" s="1">
         <v>75</v>
       </c>
-      <c r="C116" s="27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C116" s="26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B117" s="1">
         <v>76</v>
       </c>
-      <c r="C117" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D117" s="23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C117" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D117" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B118" s="1">
         <v>77</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D118" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="D118" s="9"/>
+      <c r="E118" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B119" s="1">
         <v>78</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B120" s="1">
         <v>79</v>
       </c>
-      <c r="C120" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C120" s="7"/>
+      <c r="E120" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B121" s="1">
         <v>80</v>
       </c>
-      <c r="C121" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C121" s="7"/>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B122" s="1">
         <v>81</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.15">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B123" s="1">
         <v>82</v>
       </c>
-      <c r="C123" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D123" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C123" s="7"/>
+      <c r="D123" s="9"/>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B124" s="1">
         <v>83</v>
       </c>
-      <c r="C124" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D124" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C124" s="7"/>
+      <c r="D124" s="9"/>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B125" s="1">
         <v>84</v>
       </c>
-      <c r="C125" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C125" s="7"/>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B126" s="1">
         <v>85</v>
       </c>
-      <c r="C126" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C126" s="7"/>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B127" s="1">
         <v>86</v>
       </c>
-      <c r="C127" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C127" s="7"/>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B128" s="1">
         <v>87</v>
       </c>
-      <c r="C128" s="7" t="s">
-        <v>101</v>
-      </c>
+      <c r="C128" s="7"/>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B129" s="1">
         <v>88</v>
       </c>
-      <c r="C129" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D129" s="10" t="s">
-        <v>109</v>
-      </c>
+      <c r="C129" s="7"/>
+      <c r="D129" s="9"/>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B130" s="1">
         <v>89</v>
       </c>
-      <c r="C130" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D130" s="10" t="s">
-        <v>110</v>
-      </c>
+      <c r="C130" s="7"/>
+      <c r="D130" s="9"/>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B131" s="1">
         <v>90</v>
       </c>
-      <c r="C131" s="7" t="s">
-        <v>104</v>
-      </c>
+      <c r="C131" s="7"/>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B132" s="1">
         <v>91</v>
       </c>
-      <c r="C132" s="20" t="s">
-        <v>105</v>
-      </c>
+      <c r="C132" s="19"/>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B133" s="1">
         <v>92</v>
       </c>
-      <c r="C133" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="D133" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E133" s="10" t="s">
-        <v>116</v>
+      <c r="C133" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D133" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E133" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.15">
@@ -4033,11 +3745,11 @@
         <f>B133+40</f>
         <v>132</v>
       </c>
-      <c r="C134" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D134" s="10" t="s">
-        <v>117</v>
+      <c r="C134" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D134" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.15">
@@ -4056,20 +3768,20 @@
       <c r="B139" s="1">
         <v>140</v>
       </c>
-      <c r="C139" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="D139" s="10" t="s">
-        <v>88</v>
+      <c r="C139" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D139" s="9" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B140" s="1">
-        <f>B139+1000</f>
-        <v>1140</v>
-      </c>
-      <c r="C140" s="20" t="s">
-        <v>113</v>
+        <f>B139+800</f>
+        <v>940</v>
+      </c>
+      <c r="C140" s="19" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed pointing for enemy ships
</commit_message>
<xml_diff>
--- a/Docs/Vortex Packets.xlsx
+++ b/Docs/Vortex Packets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="165" windowWidth="27795" windowHeight="14055" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="165" windowWidth="27795" windowHeight="14055"/>
   </bookViews>
   <sheets>
     <sheet name="C64 to Server" sheetId="5" r:id="rId1"/>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J89"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
@@ -791,7 +791,7 @@
     <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="3.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="2.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="2.85546875" style="1" customWidth="1"/>
     <col min="10" max="256" width="9.140625" style="1"/>
     <col min="257" max="257" width="4.85546875" style="1" customWidth="1"/>
@@ -1458,13 +1458,13 @@
       <c r="E31" s="12"/>
       <c r="F31" s="10"/>
       <c r="G31" s="17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H31" s="17">
+        <v>0</v>
+      </c>
+      <c r="I31" s="20">
         <v>1</v>
-      </c>
-      <c r="I31" s="20">
-        <v>2</v>
       </c>
       <c r="J31" s="10"/>
     </row>
@@ -1480,13 +1480,13 @@
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H32" s="17">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="I32" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J32" s="12" t="s">
         <v>34</v>
@@ -1504,13 +1504,13 @@
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H33" s="17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I33" s="20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J33" s="10"/>
     </row>
@@ -1894,7 +1894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed pointing for player ship
</commit_message>
<xml_diff>
--- a/Docs/Vortex Packets.xlsx
+++ b/Docs/Vortex Packets.xlsx
@@ -779,7 +779,7 @@
   <dimension ref="B1:J89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
@@ -1482,9 +1482,7 @@
       <c r="G32" s="17">
         <v>6</v>
       </c>
-      <c r="H32" s="17">
-        <v>255</v>
-      </c>
+      <c r="H32" s="17"/>
       <c r="I32" s="20">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Name Transmitted to Server
</commit_message>
<xml_diff>
--- a/Docs/Vortex Packets.xlsx
+++ b/Docs/Vortex Packets.xlsx
@@ -78,9 +78,6 @@
     <t>Packet Type = 1</t>
   </si>
   <si>
-    <t>Player name in PETSCII (16 Bytes)</t>
-  </si>
-  <si>
     <t>Packet Type = 2</t>
   </si>
   <si>
@@ -268,6 +265,9 @@
   </si>
   <si>
     <t>Y Center</t>
+  </si>
+  <si>
+    <t>Player name in PETSCII (15 Bytes)</t>
   </si>
 </sst>
 </file>
@@ -779,7 +779,7 @@
   <dimension ref="B1:J89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
@@ -1190,7 +1190,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>2</v>
@@ -1207,10 +1207,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.15">
@@ -1218,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.15">
@@ -1226,7 +1226,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.15">
@@ -1311,13 +1311,11 @@
       <c r="B21" s="1">
         <v>16</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="8"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B22" s="1">
-        <v>17</v>
-      </c>
-      <c r="C22" s="8"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1352,13 +1350,13 @@
         <v>0</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="12"/>
@@ -1371,10 +1369,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="12"/>
@@ -1387,7 +1385,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -1401,10 +1399,10 @@
         <v>3</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
@@ -1417,7 +1415,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="10"/>
@@ -1434,12 +1432,12 @@
         <v>8</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="10"/>
@@ -1453,7 +1451,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="10"/>
@@ -1473,10 +1471,10 @@
         <v>7</v>
       </c>
       <c r="C32" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>27</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="17">
@@ -1487,7 +1485,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.15">
@@ -1495,10 +1493,10 @@
         <v>8</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>29</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="17">
@@ -1517,7 +1515,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="12"/>
@@ -1531,7 +1529,7 @@
         <v>10</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -1545,7 +1543,7 @@
         <v>11</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
@@ -1892,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
@@ -2308,13 +2306,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="E4" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.15">
@@ -2322,10 +2320,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.15">
@@ -2363,10 +2361,10 @@
         <v>0</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
@@ -2378,7 +2376,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="22"/>
@@ -2392,7 +2390,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -2403,7 +2401,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -2414,10 +2412,10 @@
         <v>4</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
@@ -2428,7 +2426,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -2436,7 +2434,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1">
         <v>6</v>
@@ -2445,10 +2443,10 @@
         <v>3</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
@@ -2539,7 +2537,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
@@ -2550,7 +2548,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
@@ -2558,7 +2556,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="1">
         <v>16</v>
@@ -2655,7 +2653,7 @@
         <v>24</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
@@ -2666,7 +2664,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
@@ -2674,7 +2672,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="1">
         <v>26</v>
@@ -2771,7 +2769,7 @@
         <v>34</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K45" s="10"/>
       <c r="L45" s="10"/>
@@ -2782,7 +2780,7 @@
         <v>35</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
@@ -2790,7 +2788,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A47" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" s="1">
         <v>36</v>
@@ -2887,7 +2885,7 @@
         <v>44</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K55" s="10"/>
       <c r="L55" s="12"/>
@@ -2898,7 +2896,7 @@
         <v>45</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K56" s="10"/>
       <c r="L56" s="12"/>
@@ -2906,7 +2904,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A57" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" s="1">
         <v>46</v>
@@ -3003,7 +3001,7 @@
         <v>54</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
@@ -3011,12 +3009,12 @@
         <v>55</v>
       </c>
       <c r="C66" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B67" s="1">
         <v>56</v>
@@ -3089,7 +3087,7 @@
         <v>64</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
@@ -3097,12 +3095,12 @@
         <v>65</v>
       </c>
       <c r="C76" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B77" s="1">
         <v>66</v>
@@ -3170,7 +3168,7 @@
         <v>11</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I84" s="1">
         <f>24+(320/2)-(24/2)</f>
@@ -3182,10 +3180,10 @@
         <v>74</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I85" s="1">
         <f xml:space="preserve"> 50+(200/2)-(21/2)</f>
@@ -3197,7 +3195,7 @@
         <v>75</v>
       </c>
       <c r="C86" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.15">
@@ -3205,13 +3203,13 @@
         <v>76</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.15">
@@ -3219,11 +3217,11 @@
         <v>77</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D88" s="9"/>
       <c r="E88" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.15">
@@ -3231,10 +3229,10 @@
         <v>78</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.15">
@@ -3243,7 +3241,7 @@
       </c>
       <c r="C90" s="7"/>
       <c r="E90" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.15">
@@ -3252,7 +3250,7 @@
       </c>
       <c r="C91" s="7"/>
       <c r="E91" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.15">
@@ -3260,7 +3258,7 @@
         <v>81</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.15">
@@ -3332,13 +3330,13 @@
         <v>92</v>
       </c>
       <c r="C103" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E103" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="D103" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.15">
@@ -3347,10 +3345,10 @@
         <v>132</v>
       </c>
       <c r="C104" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.15">
@@ -3370,10 +3368,10 @@
         <v>140</v>
       </c>
       <c r="C109" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.15">
@@ -3382,7 +3380,7 @@
         <v>940</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>